<commit_message>
LED BOARD: 1)changed sensor side 2)all rules changed to 0.3 3)arcs on board edges
</commit_message>
<xml_diff>
--- a/Hardware/MBLv1 hardware utils.xlsx
+++ b/Hardware/MBLv1 hardware utils.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MirrorBacklighting\WC\MBLv1\Hardware\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\MBLv1\Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="10260" yWindow="0" windowWidth="27600" windowHeight="13020" activeTab="2"/>
+    <workbookView xWindow="12660" yWindow="0" windowWidth="27600" windowHeight="13020" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="BATTERY CHARGE" sheetId="3" r:id="rId2"/>
     <sheet name="USB VOLTAGE MONITORING" sheetId="4" r:id="rId3"/>
-    <sheet name="BATTERY OUT" sheetId="2" r:id="rId4"/>
+    <sheet name="THERMAL" sheetId="5" r:id="rId4"/>
+    <sheet name="BATTERY OUT" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="63">
   <si>
     <t>I nom</t>
   </si>
@@ -162,16 +163,71 @@
   </si>
   <si>
     <t>Rdown2</t>
+  </si>
+  <si>
+    <t>TRACK</t>
+  </si>
+  <si>
+    <t>width</t>
+  </si>
+  <si>
+    <t>length</t>
+  </si>
+  <si>
+    <t>copper thickness</t>
+  </si>
+  <si>
+    <t>Area</t>
+  </si>
+  <si>
+    <t>Theta</t>
+  </si>
+  <si>
+    <t>K/W</t>
+  </si>
+  <si>
+    <t>mm^2</t>
+  </si>
+  <si>
+    <t>mm</t>
+  </si>
+  <si>
+    <t>VIA</t>
+  </si>
+  <si>
+    <t>inner diameter</t>
+  </si>
+  <si>
+    <t>outer diameter</t>
+  </si>
+  <si>
+    <t>area</t>
+  </si>
+  <si>
+    <t>pcb thickness</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>m^2</t>
+  </si>
+  <si>
+    <t>COPPER</t>
+  </si>
+  <si>
+    <t>W/m/K</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -213,8 +269,33 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -236,8 +317,18 @@
         <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -260,14 +351,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -275,10 +383,18 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="4"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="5" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="6" borderId="2" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="5" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="6">
+    <cellStyle name="Accent5" xfId="5" builtinId="45"/>
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Input" xfId="4" builtinId="20"/>
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -804,7 +920,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -955,6 +1071,217 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:E17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="14.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2">
+        <v>401</v>
+      </c>
+      <c r="C2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="8">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5">
+        <f>B5/1000</f>
+        <v>1E-3</v>
+      </c>
+      <c r="E5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" s="8">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6">
+        <f>B6/1000</f>
+        <v>1E-3</v>
+      </c>
+      <c r="E6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="8">
+        <v>0.1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7">
+        <f>B7/1000</f>
+        <v>1E-4</v>
+      </c>
+      <c r="E7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8">
+        <f>B5*B7</f>
+        <v>0.1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>52</v>
+      </c>
+      <c r="D8">
+        <f>D5*D7</f>
+        <v>1.0000000000000001E-7</v>
+      </c>
+      <c r="E8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" s="11">
+        <f>D6/$B$2/D8</f>
+        <v>24.937655860349125</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>55</v>
+      </c>
+      <c r="B13">
+        <v>0.5</v>
+      </c>
+      <c r="C13" t="s">
+        <v>53</v>
+      </c>
+      <c r="D13">
+        <f>B13/1000</f>
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="E13" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>56</v>
+      </c>
+      <c r="B14">
+        <f>B13+B7</f>
+        <v>0.6</v>
+      </c>
+      <c r="C14" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14">
+        <f>B14/1000</f>
+        <v>5.9999999999999995E-4</v>
+      </c>
+      <c r="E14" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>57</v>
+      </c>
+      <c r="B15" s="7">
+        <f>3*(B14^2-B13^2)/4</f>
+        <v>8.249999999999999E-2</v>
+      </c>
+      <c r="C15" t="s">
+        <v>52</v>
+      </c>
+      <c r="D15" s="7">
+        <f>3*(D14^2-D13^2)/4</f>
+        <v>8.2499999999999965E-8</v>
+      </c>
+      <c r="E15" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>58</v>
+      </c>
+      <c r="B16">
+        <v>1.5</v>
+      </c>
+      <c r="C16" t="s">
+        <v>53</v>
+      </c>
+      <c r="D16">
+        <f>B16/1000</f>
+        <v>1.5E-3</v>
+      </c>
+      <c r="E16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="D17" s="12">
+        <f>D16/$B$2/D15</f>
+        <v>45.341192473362071</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:E15"/>
   <sheetViews>

</xml_diff>